<commit_message>
Update Team Assignment 6
</commit_message>
<xml_diff>
--- a/docs/Team Assignment 6 - Test Plan.xlsx
+++ b/docs/Team Assignment 6 - Test Plan.xlsx
@@ -58,7 +58,7 @@
     <t>write</t>
   </si>
   <si>
-    <t>steam authentication</t>
+    <t>steam authentication result</t>
   </si>
   <si>
     <t>none</t>
@@ -441,7 +441,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="23.43"/>
     <col customWidth="1" min="3" max="3" width="60.43"/>
-    <col customWidth="1" min="5" max="5" width="19.29"/>
+    <col customWidth="1" min="5" max="5" width="24.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -516,7 +516,7 @@
       <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="6" t="s">

</xml_diff>